<commit_message>
Xpath scraping is done
</commit_message>
<xml_diff>
--- a/dataSheet/getDataExcel.xlsx
+++ b/dataSheet/getDataExcel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="453">
   <si>
     <t>Actual Project Name</t>
   </si>
@@ -991,6 +991,390 @@
   </si>
   <si>
     <t>FireFlink_91585</t>
+  </si>
+  <si>
+    <t>FireFlink_01932</t>
+  </si>
+  <si>
+    <t>FireFlink_93781</t>
+  </si>
+  <si>
+    <t>FireFlink_67971</t>
+  </si>
+  <si>
+    <t>FireFlink_98663</t>
+  </si>
+  <si>
+    <t>FireFlink_93558</t>
+  </si>
+  <si>
+    <t>FireFlink_99713</t>
+  </si>
+  <si>
+    <t>FireFlink_27908</t>
+  </si>
+  <si>
+    <t>FireFlink_88820</t>
+  </si>
+  <si>
+    <t>FireFlink_58646</t>
+  </si>
+  <si>
+    <t>FireFlink_26270</t>
+  </si>
+  <si>
+    <t>FireFlink_77518</t>
+  </si>
+  <si>
+    <t>FireFlink_37757</t>
+  </si>
+  <si>
+    <t>FireFlink_87140</t>
+  </si>
+  <si>
+    <t>FireFlink_14261</t>
+  </si>
+  <si>
+    <t>FireFlink_51456</t>
+  </si>
+  <si>
+    <t>FireFlink_63540</t>
+  </si>
+  <si>
+    <t>FireFlink_98531</t>
+  </si>
+  <si>
+    <t>FireFlink_19388</t>
+  </si>
+  <si>
+    <t>FireFlink_94816</t>
+  </si>
+  <si>
+    <t>FireFlink_09536</t>
+  </si>
+  <si>
+    <t>FireFlink_47450</t>
+  </si>
+  <si>
+    <t>FireFlink_28529</t>
+  </si>
+  <si>
+    <t>FireFlink_89297</t>
+  </si>
+  <si>
+    <t>FireFlink_47417</t>
+  </si>
+  <si>
+    <t>FireFlink_06795</t>
+  </si>
+  <si>
+    <t>FireFlink_69692</t>
+  </si>
+  <si>
+    <t>FireFlink_18200</t>
+  </si>
+  <si>
+    <t>FireFlink_42520</t>
+  </si>
+  <si>
+    <t>FireFlink_02356</t>
+  </si>
+  <si>
+    <t>FireFlink_73328</t>
+  </si>
+  <si>
+    <t>FireFlink_08827</t>
+  </si>
+  <si>
+    <t>FireFlink_08556</t>
+  </si>
+  <si>
+    <t>FireFlink_81525</t>
+  </si>
+  <si>
+    <t>FireFlink_26503</t>
+  </si>
+  <si>
+    <t>FireFlink_85254</t>
+  </si>
+  <si>
+    <t>FireFlink_92121</t>
+  </si>
+  <si>
+    <t>FireFlink_71659</t>
+  </si>
+  <si>
+    <t>FireFlink_47510</t>
+  </si>
+  <si>
+    <t>FireFlink_43004</t>
+  </si>
+  <si>
+    <t>FireFlink_51746</t>
+  </si>
+  <si>
+    <t>FireFlink_14619</t>
+  </si>
+  <si>
+    <t>FireFlink_27408</t>
+  </si>
+  <si>
+    <t>FireFlink_76858</t>
+  </si>
+  <si>
+    <t>FireFlink_00969</t>
+  </si>
+  <si>
+    <t>FireFlink_11950</t>
+  </si>
+  <si>
+    <t>FireFlink_38581</t>
+  </si>
+  <si>
+    <t>FireFlink_64919</t>
+  </si>
+  <si>
+    <t>FireFlink_82099</t>
+  </si>
+  <si>
+    <t>FireFlink_77926</t>
+  </si>
+  <si>
+    <t>FireFlink_28648</t>
+  </si>
+  <si>
+    <t>FireFlink_78369</t>
+  </si>
+  <si>
+    <t>FireFlink_13397</t>
+  </si>
+  <si>
+    <t>FireFlink_55678</t>
+  </si>
+  <si>
+    <t>FireFlink_25739</t>
+  </si>
+  <si>
+    <t>FireFlink_33148</t>
+  </si>
+  <si>
+    <t>FireFlink_45717</t>
+  </si>
+  <si>
+    <t>FireFlink_55450</t>
+  </si>
+  <si>
+    <t>FireFlink_94099</t>
+  </si>
+  <si>
+    <t>FireFlink_83078</t>
+  </si>
+  <si>
+    <t>FireFlink_18163</t>
+  </si>
+  <si>
+    <t>FireFlink_16886</t>
+  </si>
+  <si>
+    <t>FireFlink_34161</t>
+  </si>
+  <si>
+    <t>FireFlink_56748</t>
+  </si>
+  <si>
+    <t>FireFlink_25609</t>
+  </si>
+  <si>
+    <t>FireFlink_61762</t>
+  </si>
+  <si>
+    <t>FireFlink_31484</t>
+  </si>
+  <si>
+    <t>FireFlink_03539</t>
+  </si>
+  <si>
+    <t>FireFlink_50146</t>
+  </si>
+  <si>
+    <t>FireFlink_89262</t>
+  </si>
+  <si>
+    <t>FireFlink_44993</t>
+  </si>
+  <si>
+    <t>FireFlink_97848</t>
+  </si>
+  <si>
+    <t>FireFlink_25224</t>
+  </si>
+  <si>
+    <t>FireFlink_43574</t>
+  </si>
+  <si>
+    <t>FireFlink_58076</t>
+  </si>
+  <si>
+    <t>FireFlink_12276</t>
+  </si>
+  <si>
+    <t>FireFlink_41085</t>
+  </si>
+  <si>
+    <t>FireFlink_18875</t>
+  </si>
+  <si>
+    <t>FireFlink_73403</t>
+  </si>
+  <si>
+    <t>FireFlink_35430</t>
+  </si>
+  <si>
+    <t>FireFlink_32872</t>
+  </si>
+  <si>
+    <t>FireFlink_54469</t>
+  </si>
+  <si>
+    <t>FireFlink_33321</t>
+  </si>
+  <si>
+    <t>FireFlink_06302</t>
+  </si>
+  <si>
+    <t>FireFlink_96908</t>
+  </si>
+  <si>
+    <t>FireFlink_51003</t>
+  </si>
+  <si>
+    <t>FireFlink_51092</t>
+  </si>
+  <si>
+    <t>FireFlink_16660</t>
+  </si>
+  <si>
+    <t>FireFlink_07148</t>
+  </si>
+  <si>
+    <t>FireFlink_00777</t>
+  </si>
+  <si>
+    <t>FireFlink_40511</t>
+  </si>
+  <si>
+    <t>FireFlink_43452</t>
+  </si>
+  <si>
+    <t>FireFlink_74147</t>
+  </si>
+  <si>
+    <t>FireFlink_22246</t>
+  </si>
+  <si>
+    <t>FireFlink_67486</t>
+  </si>
+  <si>
+    <t>FireFlink_16270</t>
+  </si>
+  <si>
+    <t>FireFlink_58585</t>
+  </si>
+  <si>
+    <t>FireFlink_48162</t>
+  </si>
+  <si>
+    <t>FireFlink_58141</t>
+  </si>
+  <si>
+    <t>FireFlink_23730</t>
+  </si>
+  <si>
+    <t>FireFlink_92862</t>
+  </si>
+  <si>
+    <t>FireFlink_76379</t>
+  </si>
+  <si>
+    <t>FireFlink_05725</t>
+  </si>
+  <si>
+    <t>FireFlink_87305</t>
+  </si>
+  <si>
+    <t>FireFlink_17912</t>
+  </si>
+  <si>
+    <t>FireFlink_02936</t>
+  </si>
+  <si>
+    <t>FireFlink_40580</t>
+  </si>
+  <si>
+    <t>FireFlink_42154</t>
+  </si>
+  <si>
+    <t>FireFlink_57740</t>
+  </si>
+  <si>
+    <t>FireFlink_84146</t>
+  </si>
+  <si>
+    <t>FireFlink_03144</t>
+  </si>
+  <si>
+    <t>FireFlink_45805</t>
+  </si>
+  <si>
+    <t>FireFlink_33287</t>
+  </si>
+  <si>
+    <t>FireFlink_86568</t>
+  </si>
+  <si>
+    <t>FireFlink_23329</t>
+  </si>
+  <si>
+    <t>FireFlink_88979</t>
+  </si>
+  <si>
+    <t>FireFlink_35639</t>
+  </si>
+  <si>
+    <t>FireFlink_00073</t>
+  </si>
+  <si>
+    <t>FireFlink_71766</t>
+  </si>
+  <si>
+    <t>FireFlink_64080</t>
+  </si>
+  <si>
+    <t>FireFlink_93137</t>
+  </si>
+  <si>
+    <t>FireFlink_50723</t>
+  </si>
+  <si>
+    <t>FireFlink_25922</t>
+  </si>
+  <si>
+    <t>FireFlink_29745</t>
+  </si>
+  <si>
+    <t>FireFlink_79172</t>
+  </si>
+  <si>
+    <t>FireFlink_79905</t>
+  </si>
+  <si>
+    <t>FireFlink_67811</t>
+  </si>
+  <si>
+    <t>FireFlink_74007</t>
+  </si>
+  <si>
+    <t>FireFlink_30136</t>
   </si>
 </sst>
 </file>
@@ -1364,7 +1748,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>324</v>
+        <v>452</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cloud integration has been done
</commit_message>
<xml_diff>
--- a/dataSheet/getDataExcel.xlsx
+++ b/dataSheet/getDataExcel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="479">
   <si>
     <t>Actual Project Name</t>
   </si>
@@ -1411,6 +1411,48 @@
   </si>
   <si>
     <t>FireFlink_79734</t>
+  </si>
+  <si>
+    <t>FireFlink_98627</t>
+  </si>
+  <si>
+    <t>FireFlink_90975</t>
+  </si>
+  <si>
+    <t>FireFlink_71553</t>
+  </si>
+  <si>
+    <t>FireFlink_43565</t>
+  </si>
+  <si>
+    <t>FireFlink_21808</t>
+  </si>
+  <si>
+    <t>FireFlink_10624</t>
+  </si>
+  <si>
+    <t>FireFlink_73385</t>
+  </si>
+  <si>
+    <t>FireFlink_81821</t>
+  </si>
+  <si>
+    <t>FireFlink_77581</t>
+  </si>
+  <si>
+    <t>FireFlink_90950</t>
+  </si>
+  <si>
+    <t>FireFlink_10498</t>
+  </si>
+  <si>
+    <t>FireFlink_59603</t>
+  </si>
+  <si>
+    <t>FireFlink_38187</t>
+  </si>
+  <si>
+    <t>FireFlink_26884</t>
   </si>
 </sst>
 </file>
@@ -1784,7 +1826,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>464</v>
+        <v>478</v>
       </c>
     </row>
   </sheetData>

</xml_diff>